<commit_message>
antes de mudar o arquivo de entrada Gaia
</commit_message>
<xml_diff>
--- a/Biostar_Catalogue/output_files/BrightStar/csv/BrightStar_estrelas_sem_ADS_Comp_e_sem_DR3.xlsx
+++ b/Biostar_Catalogue/output_files/BrightStar/csv/BrightStar_estrelas_sem_ADS_Comp_e_sem_DR3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="plotadas_no_diagrama_HR" sheetId="1" state="visible" r:id="rId3"/>
@@ -4550,8 +4550,8 @@
   </sheetPr>
   <dimension ref="A1:J353"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15321,8 +15321,8 @@
   </sheetPr>
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>